<commit_message>
Membuat proses 1 itemset
</commit_message>
<xml_diff>
--- a/public/DataTransaction/Sample Data 1.xlsx
+++ b/public/DataTransaction/Sample Data 1.xlsx
@@ -15,7 +15,7 @@
     <sheet name="AGUSTUS 2021" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'AGUSTUS 2021'!$C$1:$C$302</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'AGUSTUS 2021'!$C$1:$C$300</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,57 +27,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
   <si>
-    <t>TMB02590</t>
+    <t>JACK DANIEL</t>
   </si>
   <si>
-    <t>TMB02591</t>
+    <t>ABSOLUT BLUE</t>
   </si>
   <si>
-    <t>TMB02592</t>
+    <t>SINGLETON 12 YO</t>
   </si>
   <si>
-    <t>TMB02593</t>
+    <t>BACARDI</t>
   </si>
   <si>
-    <t>TMB02594</t>
+    <t>CAPTAIN MORGAN</t>
   </si>
   <si>
-    <t>TMB02595</t>
+    <t>T1</t>
   </si>
   <si>
-    <t>TMB02596</t>
+    <t>T2</t>
   </si>
   <si>
-    <t>TMB02597</t>
+    <t>T3</t>
   </si>
   <si>
-    <t>CAPTAINMORGANGOLDRUM750ML</t>
+    <t>T4</t>
   </si>
   <si>
-    <t>APEROLAPERITIVO700ML</t>
-  </si>
-  <si>
-    <t>JJMCWILLIAMSHIRAZ750ML</t>
-  </si>
-  <si>
-    <t>G7SAUVIGNONBLANC750ML</t>
-  </si>
-  <si>
-    <t>JJMCWILLIAMPINOTGRIGIO750ML</t>
-  </si>
-  <si>
-    <t>ISOLAROSSOBULELENGCOAST750ML</t>
-  </si>
-  <si>
-    <t>JOSECUERVOESPECIALSILVER750ML</t>
-  </si>
-  <si>
-    <t>SMIRNOFFVODKA750ML</t>
-  </si>
-  <si>
-    <t>CAPTAINMORGANWHITERUM750ML</t>
+    <t>T5</t>
   </si>
 </sst>
 </file>
@@ -485,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N375"/>
+  <dimension ref="A1:N373"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -513,22 +492,19 @@
         <v>44410</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" s="8">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="E1" s="8">
-        <v>203057.8</v>
+        <v>0</v>
       </c>
       <c r="F1" s="4">
-        <v>5685618.3999999994</v>
-      </c>
-      <c r="G1" s="4">
-        <v>5685618.3999999994</v>
+        <v>0</v>
       </c>
       <c r="H1" s="6"/>
       <c r="I1" s="8"/>
@@ -536,39 +512,44 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="C2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
       <c r="H2" s="6"/>
       <c r="I2" s="8"/>
       <c r="J2" s="9"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
-        <v>44410</v>
-      </c>
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="8">
-        <v>2</v>
-      </c>
       <c r="E3" s="8">
-        <v>414000.18</v>
+        <v>0</v>
       </c>
       <c r="F3" s="4">
-        <v>828000.36</v>
+        <v>0</v>
       </c>
       <c r="G3" s="4">
-        <v>828000.36</v>
+        <v>0</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="8"/>
@@ -593,22 +574,19 @@
         <v>44410</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D5" s="8">
         <v>1</v>
       </c>
       <c r="E5" s="8">
-        <v>414000.18</v>
+        <v>0</v>
       </c>
       <c r="F5" s="4">
-        <v>414000.18</v>
-      </c>
-      <c r="G5" s="4">
-        <v>414000.18</v>
+        <v>0</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="8"/>
@@ -619,9 +597,21 @@
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="C6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
       <c r="H6" s="6"/>
       <c r="I6" s="8"/>
       <c r="J6" s="9"/>
@@ -629,27 +619,11 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
-        <v>44410</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="8">
-        <v>6</v>
-      </c>
-      <c r="E7" s="8">
-        <v>414000.18</v>
-      </c>
-      <c r="F7" s="4">
-        <v>2484001.08</v>
-      </c>
-      <c r="G7" s="4">
-        <v>2484001.08</v>
-      </c>
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
       <c r="H7" s="6"/>
       <c r="I7" s="8"/>
       <c r="J7" s="9"/>
@@ -657,11 +631,24 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="A8" s="5">
+        <v>44410</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
       <c r="H8" s="6"/>
       <c r="I8" s="8"/>
       <c r="J8" s="9"/>
@@ -669,26 +656,19 @@
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
-        <v>44410</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>4</v>
-      </c>
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="7" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D9" s="8">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E9" s="8">
-        <v>195000.3</v>
+        <v>0</v>
       </c>
       <c r="F9" s="4">
-        <v>1560002.4</v>
-      </c>
-      <c r="G9" s="4">
-        <v>1560002.4</v>
+        <v>0</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="8"/>
@@ -699,9 +679,21 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="C10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="8"/>
       <c r="J10" s="9"/>
@@ -709,24 +701,11 @@
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
-        <v>44410</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="8">
-        <v>1</v>
-      </c>
-      <c r="E11" s="8">
-        <v>257999.5</v>
-      </c>
-      <c r="F11" s="4">
-        <v>257999.5</v>
-      </c>
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
       <c r="H11" s="6"/>
       <c r="I11" s="8"/>
       <c r="J11" s="9"/>
@@ -734,19 +713,23 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
+      <c r="A12" s="5">
+        <v>44410</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="C12" s="7" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D12" s="8">
         <v>1</v>
       </c>
       <c r="E12" s="8">
-        <v>248000.5</v>
+        <v>0</v>
       </c>
       <c r="F12" s="4">
-        <v>248000.5</v>
+        <v>0</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="8"/>
@@ -758,16 +741,16 @@
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D13" s="8">
         <v>1</v>
       </c>
       <c r="E13" s="8">
-        <v>257999.5</v>
+        <v>0</v>
       </c>
       <c r="F13" s="4">
-        <v>257999.5</v>
+        <v>0</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="8"/>
@@ -779,19 +762,16 @@
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D14" s="8">
         <v>1</v>
       </c>
       <c r="E14" s="8">
-        <v>195000.3</v>
+        <v>0</v>
       </c>
       <c r="F14" s="4">
-        <v>195000.3</v>
-      </c>
-      <c r="G14" s="4">
-        <v>958999.8</v>
+        <v>0</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="8"/>
@@ -802,9 +782,21 @@
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="C15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="8">
+        <v>1</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
       <c r="H15" s="6"/>
       <c r="I15" s="8"/>
       <c r="J15" s="9"/>
@@ -812,24 +804,11 @@
       <c r="N15" s="1"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
-        <v>44410</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="8">
-        <v>6</v>
-      </c>
-      <c r="E16" s="8">
-        <v>621900.17999999993</v>
-      </c>
-      <c r="F16" s="4">
-        <v>3731401.0799999996</v>
-      </c>
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
       <c r="H16" s="6"/>
       <c r="I16" s="8"/>
       <c r="J16" s="9"/>
@@ -837,22 +816,23 @@
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="5">
+        <v>44410</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="C17" s="7" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D17" s="8">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E17" s="8">
-        <v>184286.3</v>
+        <v>0</v>
       </c>
       <c r="F17" s="4">
-        <v>1290004.0999999999</v>
-      </c>
-      <c r="G17" s="4">
-        <v>5021405.18</v>
+        <v>0</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="8"/>
@@ -863,9 +843,21 @@
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="C18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="8">
+        <v>1</v>
+      </c>
+      <c r="E18" s="8">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0</v>
+      </c>
       <c r="H18" s="6"/>
       <c r="I18" s="8"/>
       <c r="J18" s="9"/>
@@ -873,24 +865,11 @@
       <c r="N18" s="1"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="5">
-        <v>44411</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="8">
-        <v>7</v>
-      </c>
-      <c r="E19" s="8">
-        <v>184286.3</v>
-      </c>
-      <c r="F19" s="4">
-        <v>1290004.0999999999</v>
-      </c>
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
       <c r="H19" s="6"/>
       <c r="I19" s="8"/>
       <c r="J19" s="9"/>
@@ -898,28 +877,8 @@
       <c r="N19" s="1"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="8">
-        <v>1</v>
-      </c>
-      <c r="E20" s="8">
-        <v>236900.4</v>
-      </c>
-      <c r="F20" s="4">
-        <v>236900.4</v>
-      </c>
-      <c r="G20" s="4">
-        <v>1526904.4999999998</v>
-      </c>
-      <c r="H20" s="6"/>
+      <c r="C20" s="7"/>
       <c r="I20" s="8"/>
-      <c r="J20" s="9"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
@@ -927,15 +886,17 @@
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="9"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="7"/>
-      <c r="I22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
@@ -1748,13 +1709,7 @@
       <c r="I112" s="1"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A113" s="5"/>
-      <c r="B113" s="6"/>
       <c r="C113" s="7"/>
-      <c r="D113" s="8"/>
-      <c r="E113" s="8"/>
-      <c r="H113" s="10"/>
-      <c r="I113" s="1"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" s="5"/>
@@ -1766,7 +1721,13 @@
       <c r="I114" s="1"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A115" s="5"/>
+      <c r="B115" s="6"/>
       <c r="C115" s="7"/>
+      <c r="D115" s="8"/>
+      <c r="E115" s="8"/>
+      <c r="H115" s="10"/>
+      <c r="I115" s="1"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" s="5"/>
@@ -2264,13 +2225,7 @@
       <c r="I170" s="1"/>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A171" s="5"/>
-      <c r="B171" s="6"/>
       <c r="C171" s="7"/>
-      <c r="D171" s="8"/>
-      <c r="E171" s="8"/>
-      <c r="H171" s="10"/>
-      <c r="I171" s="1"/>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A172" s="5"/>
@@ -2282,7 +2237,13 @@
       <c r="I172" s="1"/>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A173" s="5"/>
+      <c r="B173" s="6"/>
       <c r="C173" s="7"/>
+      <c r="D173" s="8"/>
+      <c r="E173" s="8"/>
+      <c r="H173" s="10"/>
+      <c r="I173" s="1"/>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A174" s="5"/>
@@ -2843,13 +2804,7 @@
       <c r="I235" s="1"/>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A236" s="5"/>
-      <c r="B236" s="6"/>
       <c r="C236" s="7"/>
-      <c r="D236" s="8"/>
-      <c r="E236" s="8"/>
-      <c r="H236" s="10"/>
-      <c r="I236" s="1"/>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A237" s="5"/>
@@ -2861,7 +2816,13 @@
       <c r="I237" s="1"/>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A238" s="5"/>
+      <c r="B238" s="6"/>
       <c r="C238" s="7"/>
+      <c r="D238" s="8"/>
+      <c r="E238" s="8"/>
+      <c r="H238" s="10"/>
+      <c r="I238" s="1"/>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A239" s="5"/>
@@ -3382,25 +3343,17 @@
       <c r="C296" s="7"/>
       <c r="D296" s="8"/>
       <c r="E296" s="8"/>
-      <c r="H296" s="10"/>
-      <c r="I296" s="1"/>
+      <c r="H296" s="1"/>
     </row>
     <row r="297" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A297" s="5"/>
-      <c r="B297" s="6"/>
       <c r="C297" s="7"/>
       <c r="D297" s="8"/>
       <c r="E297" s="8"/>
-      <c r="H297" s="10"/>
-      <c r="I297" s="1"/>
     </row>
     <row r="298" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A298" s="5"/>
-      <c r="B298" s="6"/>
       <c r="C298" s="7"/>
       <c r="D298" s="8"/>
       <c r="E298" s="8"/>
-      <c r="H298" s="1"/>
     </row>
     <row r="299" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C299" s="7"/>
@@ -3414,16 +3367,24 @@
     </row>
     <row r="301" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C301" s="7"/>
-      <c r="D301" s="8"/>
-      <c r="E301" s="8"/>
     </row>
     <row r="302" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A302" s="5"/>
+      <c r="B302" s="6"/>
       <c r="C302" s="7"/>
       <c r="D302" s="8"/>
       <c r="E302" s="8"/>
+      <c r="H302" s="10"/>
+      <c r="I302" s="1"/>
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A303" s="5"/>
+      <c r="B303" s="6"/>
       <c r="C303" s="7"/>
+      <c r="D303" s="8"/>
+      <c r="E303" s="8"/>
+      <c r="H303" s="10"/>
+      <c r="I303" s="1"/>
     </row>
     <row r="304" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A304" s="5"/>
@@ -3975,13 +3936,7 @@
       <c r="I364" s="1"/>
     </row>
     <row r="365" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A365" s="5"/>
-      <c r="B365" s="6"/>
       <c r="C365" s="7"/>
-      <c r="D365" s="8"/>
-      <c r="E365" s="8"/>
-      <c r="H365" s="10"/>
-      <c r="I365" s="1"/>
     </row>
     <row r="366" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A366" s="5"/>
@@ -3993,7 +3948,13 @@
       <c r="I366" s="1"/>
     </row>
     <row r="367" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A367" s="5"/>
+      <c r="B367" s="6"/>
       <c r="C367" s="7"/>
+      <c r="D367" s="8"/>
+      <c r="E367" s="8"/>
+      <c r="H367" s="10"/>
+      <c r="I367" s="1"/>
     </row>
     <row r="368" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A368" s="5"/>
@@ -4014,34 +3975,16 @@
       <c r="I369" s="1"/>
     </row>
     <row r="370" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A370" s="5"/>
-      <c r="B370" s="6"/>
       <c r="C370" s="7"/>
-      <c r="D370" s="8"/>
-      <c r="E370" s="8"/>
-      <c r="H370" s="10"/>
-      <c r="I370" s="1"/>
     </row>
     <row r="371" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A371" s="5"/>
-      <c r="B371" s="6"/>
       <c r="C371" s="7"/>
-      <c r="D371" s="8"/>
-      <c r="E371" s="8"/>
-      <c r="H371" s="10"/>
-      <c r="I371" s="1"/>
     </row>
     <row r="372" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C372" s="7"/>
     </row>
     <row r="373" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C373" s="7"/>
-    </row>
-    <row r="374" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C374" s="7"/>
-    </row>
-    <row r="375" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C375" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>